<commit_message>
Made first csv for shifted lat longs
</commit_message>
<xml_diff>
--- a/docs/OnceWas_latlong_all_nums_shifted.xlsx
+++ b/docs/OnceWas_latlong_all_nums_shifted.xlsx
@@ -3785,7 +3785,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -4284,7 +4284,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -4623,12 +4623,12 @@
   <dimension ref="A1:P339"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J337" sqref="J337"/>
+      <selection sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="16" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" style="5" bestFit="1" customWidth="1"/>

</xml_diff>